<commit_message>
Uniandes 2023: Rename tone disc folder
</commit_message>
<xml_diff>
--- a/Especial_Uniandes_2023/3. Programa de curso/Ideas curso.xlsx
+++ b/Especial_Uniandes_2023/3. Programa de curso/Ideas curso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\Especial_Uniandes_2023\3. Programa de curso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C43A46-09A0-4970-9109-140222CFFA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E31873D-F26A-49F6-A970-07F85B6E4D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B3736183-08CD-48DA-B926-7FA45C0C5222}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
   <si>
     <t>Relación música lenguaje</t>
   </si>
@@ -344,6 +344,9 @@
   <si>
     <t>Bases review https://doi.org/10.1152/physrev.00006.2011</t>
   </si>
+  <si>
+    <t>Estructura de frases https://doi.org/10.1073/pnas.1018711108</t>
+  </si>
 </sst>
 </file>
 
@@ -584,7 +587,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -606,9 +609,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -940,14 +940,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{808D17E8-0F73-4294-A09C-161321AB1AF7}">
   <dimension ref="A2:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="175.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="138.28515625" customWidth="1"/>
     <col min="3" max="3" width="53.28515625" customWidth="1"/>
     <col min="4" max="4" width="53.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1114,7 +1114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>35</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>39</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
         <v>41</v>
       </c>
@@ -1221,10 +1221,10 @@
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="19"/>
+      <c r="B50" s="18"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
@@ -1275,16 +1275,16 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="18" t="s">
+      <c r="A57" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B57" s="19"/>
+      <c r="B57" s="18"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
         <v>7</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="12" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1292,7 +1292,7 @@
       <c r="A59" s="11">
         <v>8</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="12" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1300,7 +1300,7 @@
       <c r="A60" s="11">
         <v>9</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="12" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1308,7 +1308,7 @@
       <c r="A61" s="11">
         <v>10</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="12" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1321,10 +1321,10 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="18" t="s">
+      <c r="A63" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="19"/>
+      <c r="B63" s="18"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
@@ -1363,11 +1363,14 @@
       <c r="A67" s="11">
         <v>15</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="12" t="s">
         <v>56</v>
       </c>
       <c r="C67" t="s">
         <v>64</v>
+      </c>
+      <c r="D67" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>